<commit_message>
updated design specification so the tabulated pseudo code is in it
</commit_message>
<xml_diff>
--- a/Pseudo Code/getTrained.xlsx
+++ b/Pseudo Code/getTrained.xlsx
@@ -499,14 +499,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.5703125" customWidth="1"/>
-    <col min="2" max="2" width="59.28515625" customWidth="1"/>
+    <col min="2" max="2" width="52.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">

</xml_diff>